<commit_message>
Creation of Figures and Tables and text of paper
</commit_message>
<xml_diff>
--- a/Analysis/Output/Results.xlsx
+++ b/Analysis/Output/Results.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\Leili_Anna_EPA\Analysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2DCAC9-B550-4EF1-A106-F9A0C1114DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F333BD-C480-4B5D-A894-083AA1BE1891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E6D7BEF-83A0-4049-80E6-42C5CBAED8F0}"/>
+    <workbookView xWindow="16395" yWindow="5655" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{0E6D7BEF-83A0-4049-80E6-42C5CBAED8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Table 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="146">
   <si>
     <t>coef</t>
   </si>
@@ -388,6 +389,93 @@
   </si>
   <si>
     <t>Region 10</t>
+  </si>
+  <si>
+    <t>npv</t>
+  </si>
+  <si>
+    <t>SITE_SCORE</t>
+  </si>
+  <si>
+    <t>federal</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Desscription</t>
+  </si>
+  <si>
+    <t>Completed Cleanup</t>
+  </si>
+  <si>
+    <t>Duration of Cleanup (days)</t>
+  </si>
+  <si>
+    <t>NPV ($100,000)</t>
+  </si>
+  <si>
+    <t>Hazard Ranking Score</t>
+  </si>
+  <si>
+    <t>Federally Owned Sites</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Percentage Minority</t>
+  </si>
+  <si>
+    <t>Percentage over 65 years</t>
+  </si>
+  <si>
+    <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Percentage with no High School Degree</t>
+  </si>
+  <si>
+    <t>Percentage with High School Degree or GED</t>
+  </si>
+  <si>
+    <t>Percentage with a College Degree</t>
+  </si>
+  <si>
+    <t>Voter Participation Rate</t>
+  </si>
+  <si>
+    <t>Democratic Representative</t>
+  </si>
+  <si>
+    <t>minc</t>
+  </si>
+  <si>
+    <t>Median Income ($)</t>
+  </si>
+  <si>
+    <t>Table 1: Summary Statistics for Superfund Sites and Census Data within 1 Mile of Site</t>
+  </si>
+  <si>
+    <t>Variable (N = 1398)</t>
+  </si>
+  <si>
+    <t>v_low_haz</t>
+  </si>
+  <si>
+    <t>low_haz</t>
+  </si>
+  <si>
+    <t>hg_haz</t>
+  </si>
+  <si>
+    <t>v_hg_haz</t>
+  </si>
+  <si>
+    <t>Community Advisory Group</t>
   </si>
 </sst>
 </file>
@@ -398,8 +486,16 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -415,7 +511,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -441,11 +537,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -455,17 +571,23 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,30 +936,30 @@
       <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="9" t="s">
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="9" t="s">
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -3176,7 +3298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FFCE75-4ACE-4C52-934B-831B375EE130}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -3206,22 +3328,22 @@
       <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3235,16 +3357,16 @@
       <c r="J2" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="10">
         <v>5007.7439999999997</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="10">
         <v>2816.4769999999999</v>
       </c>
       <c r="M2">
         <v>111</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="11">
         <v>11531</v>
       </c>
     </row>
@@ -3252,19 +3374,19 @@
       <c r="A3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>1026</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>1994.181</v>
       </c>
       <c r="D3">
         <v>7.01</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>1990</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>2010</v>
       </c>
       <c r="I3" t="s">
@@ -3290,19 +3412,19 @@
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>1026</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>5007.7439999999997</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>2816.4769999999999</v>
       </c>
       <c r="E4">
         <v>111</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>11531</v>
       </c>
       <c r="I4" t="s">
@@ -3328,7 +3450,7 @@
       <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>1026</v>
       </c>
       <c r="C5">
@@ -3366,19 +3488,19 @@
       <c r="A6" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>1026</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>1993.3209999999999</v>
       </c>
       <c r="D6">
         <v>7.835</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>1986</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>2013</v>
       </c>
       <c r="I6" t="s">
@@ -3404,7 +3526,7 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>1026</v>
       </c>
       <c r="C7">
@@ -3422,7 +3544,7 @@
       <c r="I7" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="11" t="s">
         <v>72</v>
       </c>
       <c r="K7">
@@ -3442,7 +3564,7 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>1026</v>
       </c>
       <c r="C8">
@@ -3460,7 +3582,7 @@
       <c r="I8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="11" t="s">
         <v>73</v>
       </c>
       <c r="K8">
@@ -3480,7 +3602,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>1026</v>
       </c>
       <c r="C9">
@@ -3498,7 +3620,7 @@
       <c r="I9" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="11" t="s">
         <v>75</v>
       </c>
       <c r="K9">
@@ -3518,7 +3640,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="11">
         <v>1026</v>
       </c>
       <c r="C10">
@@ -3536,7 +3658,7 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="11" t="s">
         <v>76</v>
       </c>
       <c r="K10">
@@ -3556,7 +3678,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="11">
         <v>1026</v>
       </c>
       <c r="C11">
@@ -3574,7 +3696,7 @@
       <c r="I11" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="11" t="s">
         <v>77</v>
       </c>
       <c r="K11">
@@ -3594,7 +3716,7 @@
       <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <v>1026</v>
       </c>
       <c r="C12">
@@ -3612,7 +3734,7 @@
       <c r="I12" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="11" t="s">
         <v>79</v>
       </c>
       <c r="K12">
@@ -3632,7 +3754,7 @@
       <c r="A13" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>1026</v>
       </c>
       <c r="C13">
@@ -3650,7 +3772,7 @@
       <c r="I13" t="s">
         <v>81</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="11" t="s">
         <v>82</v>
       </c>
       <c r="K13">
@@ -3670,7 +3792,7 @@
       <c r="A14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>1026</v>
       </c>
       <c r="C14">
@@ -3688,7 +3810,7 @@
       <c r="I14" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="11" t="s">
         <v>84</v>
       </c>
       <c r="K14">
@@ -3708,7 +3830,7 @@
       <c r="A15" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>1026</v>
       </c>
       <c r="C15">
@@ -3726,7 +3848,7 @@
       <c r="I15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="11" t="s">
         <v>85</v>
       </c>
       <c r="K15">
@@ -3746,7 +3868,7 @@
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>1026</v>
       </c>
       <c r="C16">
@@ -3764,7 +3886,7 @@
       <c r="I16" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="K16">
@@ -3784,7 +3906,7 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>1026</v>
       </c>
       <c r="C17">
@@ -3802,7 +3924,7 @@
       <c r="I17" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="11" t="s">
         <v>89</v>
       </c>
       <c r="K17">
@@ -3822,7 +3944,7 @@
       <c r="A18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>1026</v>
       </c>
       <c r="C18">
@@ -3840,7 +3962,7 @@
       <c r="I18" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="11" t="s">
         <v>91</v>
       </c>
       <c r="K18">
@@ -3860,7 +3982,7 @@
       <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>1026</v>
       </c>
       <c r="C19">
@@ -3878,7 +4000,7 @@
       <c r="I19" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="11" t="s">
         <v>92</v>
       </c>
       <c r="K19">
@@ -3898,7 +4020,7 @@
       <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>1026</v>
       </c>
       <c r="C20">
@@ -3913,22 +4035,22 @@
       <c r="F20">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="13">
         <v>4736.4080000000004</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="13">
         <v>2489.8290000000002</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="9">
         <v>123.898</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="13">
         <v>35682</v>
       </c>
     </row>
@@ -3936,7 +4058,7 @@
       <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>1026</v>
       </c>
       <c r="C21">
@@ -3965,7 +4087,7 @@
       <c r="A22" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>1026</v>
       </c>
       <c r="C22">
@@ -3980,7 +4102,7 @@
       <c r="F22">
         <v>0.36599999999999999</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="11" t="s">
         <v>98</v>
       </c>
       <c r="K22">
@@ -3995,7 +4117,7 @@
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="11">
         <v>1026</v>
       </c>
       <c r="C23">
@@ -4010,7 +4132,7 @@
       <c r="F23">
         <v>0.27700000000000002</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="11" t="s">
         <v>99</v>
       </c>
       <c r="K23">
@@ -4025,7 +4147,7 @@
       <c r="A24" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="11">
         <v>1026</v>
       </c>
       <c r="C24">
@@ -4048,22 +4170,22 @@
       <c r="A25" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="11">
         <v>1026</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="10">
         <v>35573.94</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="10">
         <v>15306.51</v>
       </c>
       <c r="E25">
         <v>759.79600000000005</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="10">
         <v>113618</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="11" t="s">
         <v>102</v>
       </c>
       <c r="K25">
@@ -4078,22 +4200,22 @@
       <c r="A26" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="11">
         <v>1026</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="10">
         <v>4736.4080000000004</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="10">
         <v>2489.8290000000002</v>
       </c>
       <c r="E26">
         <v>123.898</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <v>35682</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="11" t="s">
         <v>103</v>
       </c>
       <c r="K26">
@@ -4108,7 +4230,7 @@
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>1026</v>
       </c>
       <c r="C27">
@@ -4123,7 +4245,7 @@
       <c r="F27">
         <v>11.641</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="11" t="s">
         <v>104</v>
       </c>
       <c r="K27">
@@ -4138,7 +4260,7 @@
       <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="11">
         <v>1026</v>
       </c>
       <c r="C28">
@@ -4153,7 +4275,7 @@
       <c r="F28">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="11" t="s">
         <v>105</v>
       </c>
       <c r="K28">
@@ -4171,7 +4293,7 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="11" t="s">
         <v>107</v>
       </c>
       <c r="K30">
@@ -4183,7 +4305,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="11" t="s">
         <v>108</v>
       </c>
       <c r="K31">
@@ -4195,7 +4317,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="11" t="s">
         <v>109</v>
       </c>
       <c r="K32">
@@ -4207,7 +4329,7 @@
       </c>
     </row>
     <row r="33" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="11" t="s">
         <v>110</v>
       </c>
       <c r="K33">
@@ -4219,7 +4341,7 @@
       </c>
     </row>
     <row r="34" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="11" t="s">
         <v>111</v>
       </c>
       <c r="K34">
@@ -4231,7 +4353,7 @@
       </c>
     </row>
     <row r="35" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="11" t="s">
         <v>112</v>
       </c>
       <c r="K35">
@@ -4243,7 +4365,7 @@
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="11" t="s">
         <v>113</v>
       </c>
       <c r="K36">
@@ -4255,7 +4377,7 @@
       </c>
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="11" t="s">
         <v>114</v>
       </c>
       <c r="K37">
@@ -4267,7 +4389,7 @@
       </c>
     </row>
     <row r="38" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="11" t="s">
         <v>115</v>
       </c>
       <c r="K38">
@@ -4279,7 +4401,7 @@
       </c>
     </row>
     <row r="39" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J39" s="13" t="s">
+      <c r="J39" s="11" t="s">
         <v>116</v>
       </c>
       <c r="K39">
@@ -5872,4 +5994,736 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54B0BE8-058A-48DD-9A7F-F6B87805489C}">
+  <dimension ref="A1:I43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5389</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3039</v>
+      </c>
+      <c r="E4" s="2">
+        <v>111</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12540</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="2">
+        <v>143.9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>599.4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>14760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43.14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8.6630000000000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>28.51</v>
+      </c>
+      <c r="F6" s="2">
+        <v>84.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.1196</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.3246</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.4380000000000001E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4799</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2488</v>
+      </c>
+      <c r="E9" s="2">
+        <v>69.94</v>
+      </c>
+      <c r="F9" s="2">
+        <v>35680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.1434</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1772</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.9829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.1103</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.53469999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.5419999999999997E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5.3249999999999999E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.519E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.29759999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6.5809999999999994E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4.5359999999999998E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.2722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.43919999999999998</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8.0509999999999998E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.7570000000000001E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.82150000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.1076</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7.3179999999999995E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.54979999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="2">
+        <v>30870</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15560</v>
+      </c>
+      <c r="E16" s="2">
+        <v>275.2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>113600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.54659999999999997</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.50290000000000001</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>0.68189999999999995</v>
+      </c>
+      <c r="C24">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <v>5389</v>
+      </c>
+      <c r="C25">
+        <v>3039</v>
+      </c>
+      <c r="D25">
+        <v>111</v>
+      </c>
+      <c r="E25">
+        <v>12540</v>
+      </c>
+      <c r="F25">
+        <f>B25/365</f>
+        <v>14.764383561643836</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:I25" si="0">C25/365</f>
+        <v>8.3260273972602743</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0.30410958904109592</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>34.356164383561641</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26">
+        <v>143.9</v>
+      </c>
+      <c r="C26">
+        <v>599.4</v>
+      </c>
+      <c r="D26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E26">
+        <v>14760</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27">
+        <v>43.14</v>
+      </c>
+      <c r="C27">
+        <v>8.6630000000000003</v>
+      </c>
+      <c r="D27">
+        <v>28.51</v>
+      </c>
+      <c r="E27">
+        <v>84.91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28">
+        <v>0.1196</v>
+      </c>
+      <c r="C28">
+        <v>0.3246</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>3.4380000000000001E-2</v>
+      </c>
+      <c r="C29">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>4799</v>
+      </c>
+      <c r="C30">
+        <v>2488</v>
+      </c>
+      <c r="D30">
+        <v>69.94</v>
+      </c>
+      <c r="E30">
+        <v>35680</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>0.1434</v>
+      </c>
+      <c r="C31">
+        <v>0.1772</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.9829</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>0.1103</v>
+      </c>
+      <c r="C32">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.53469999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>5.5419999999999997E-2</v>
+      </c>
+      <c r="C33">
+        <v>5.3249999999999999E-2</v>
+      </c>
+      <c r="D33">
+        <v>1.519E-3</v>
+      </c>
+      <c r="E33">
+        <v>0.29759999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34">
+        <v>6.5809999999999994E-2</v>
+      </c>
+      <c r="C34">
+        <v>4.5359999999999998E-2</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0.2722</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>0.43919999999999998</v>
+      </c>
+      <c r="C35">
+        <v>8.0509999999999998E-2</v>
+      </c>
+      <c r="D35">
+        <v>2.7570000000000001E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.82150000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>0.1076</v>
+      </c>
+      <c r="C36">
+        <v>7.3179999999999995E-2</v>
+      </c>
+      <c r="D36">
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="E36">
+        <v>0.54979999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37">
+        <v>30870</v>
+      </c>
+      <c r="C37">
+        <v>15560</v>
+      </c>
+      <c r="D37">
+        <v>275.2</v>
+      </c>
+      <c r="E37">
+        <v>113600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>0.54659999999999997</v>
+      </c>
+      <c r="C38">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D38">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E38">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39">
+        <v>0.50290000000000001</v>
+      </c>
+      <c r="C39">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C40">
+        <v>0.4415</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="C41">
+        <v>0.45129999999999998</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42">
+        <v>0.32090000000000002</v>
+      </c>
+      <c r="C42">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="C43">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>